<commit_message>
test run for gitlab
</commit_message>
<xml_diff>
--- a/project/database.xlsx
+++ b/project/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mc200205075\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6170AFF5-A0D0-4C20-893B-44AC26A99F55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FA4D97-203A-42A5-9997-E9917C76FA91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2490" windowWidth="25440" windowHeight="10770" xr2:uid="{EAF9472E-1713-4124-834B-8A8D589258F6}"/>
+    <workbookView xWindow="2280" yWindow="1170" windowWidth="25440" windowHeight="10770" xr2:uid="{EAF9472E-1713-4124-834B-8A8D589258F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t xml:space="preserve">Actors </t>
   </si>
@@ -45,12 +45,6 @@
     <t>Student</t>
   </si>
   <si>
-    <t xml:space="preserve">USER </t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Student_id</t>
   </si>
   <si>
-    <t>actor_id</t>
-  </si>
-  <si>
     <t>user_roles</t>
   </si>
   <si>
@@ -90,12 +81,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
@@ -115,6 +100,66 @@
   </si>
   <si>
     <t xml:space="preserve">Form Registration </t>
+  </si>
+  <si>
+    <t>status(int)</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form </t>
+  </si>
+  <si>
+    <t>html tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">method </t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submit </t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>addition of admin</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>creation of users table</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>INSERT into users (username, password) VALUES ('admin', 'admin123')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation of user_role </t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS user_roles(id INT NOT NULL AUTO_INCREMENT PRIMARY KEY, roles_name VARCHAR(12));</t>
+  </si>
+  <si>
+    <t>CREATE IF NOT EXISTS TABLE users(id INT NOT NULL AUTO_INCREMENT PRIMARY KEY, roles_id INT NOT NULL, username VARCHAR(50), password VARCHAR(50), status TINYINT(1) NOT NULL DEFAULT 0, created_at DATETIME DEFAULT CURRENT_TIMESTAMP, approved_by INT NOT NULL, updated_at TIMESTAMP DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP, updated_by INT)</t>
   </si>
 </sst>
 </file>
@@ -466,14 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B70D8BC-7D48-4677-8A8E-4578723C7915}">
-  <dimension ref="B4:U19"/>
+  <dimension ref="B4:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
@@ -484,18 +531,18 @@
   <sheetData>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -503,10 +550,10 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -517,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -526,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S7">
         <v>2</v>
@@ -537,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -546,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S8">
         <v>3</v>
@@ -557,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -566,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
@@ -574,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
@@ -582,43 +629,37 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" t="s">
         <v>19</v>
       </c>
-      <c r="M12" t="s">
+      <c r="S12" t="s">
         <v>20</v>
       </c>
-      <c r="N12" t="s">
+      <c r="T12" t="s">
         <v>21</v>
       </c>
-      <c r="O12" t="s">
+      <c r="U12" t="s">
         <v>22</v>
-      </c>
-      <c r="P12" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" t="s">
-        <v>24</v>
-      </c>
-      <c r="S12" t="s">
-        <v>25</v>
-      </c>
-      <c r="T12" t="s">
-        <v>26</v>
-      </c>
-      <c r="U12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
@@ -628,8 +669,29 @@
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13">
-        <v>1</v>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
@@ -639,8 +701,8 @@
       <c r="J14">
         <v>2</v>
       </c>
-      <c r="K14">
-        <v>1</v>
+      <c r="O14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
@@ -650,13 +712,78 @@
       <c r="J15">
         <v>3</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
         <v>29</v>
+      </c>
+      <c r="K20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>